<commit_message>
fileCls imports all spreadsheets
</commit_message>
<xml_diff>
--- a/test/Sample questions spreadsheet.xlsx
+++ b/test/Sample questions spreadsheet.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sample" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Another sample" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Sample spreadsheet for fpdt testing</t>
   </si>
@@ -26,6 +27,9 @@
   </si>
   <si>
     <t>Temperature 3 (F)</t>
+  </si>
+  <si>
+    <t>Sample spreadsheet for fpdt testing, second sheet</t>
   </si>
 </sst>
 </file>
@@ -81,6 +85,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -136,6 +144,95 @@
       <c r="A7" s="2">
         <v>5.0</v>
       </c>
+      <c r="C7" s="2">
+        <v>175.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>10.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2">

</xml_diff>